<commit_message>
change surface for a string
</commit_message>
<xml_diff>
--- a/static/files/cadastre.xlsx
+++ b/static/files/cadastre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D6468-AE64-0046-A33E-53A6891646EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5DF01B-7FDC-884E-868A-EB3E700A4D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31060" yWindow="3060" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -262,8 +262,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,7 +581,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
change surface for a string (#39)
</commit_message>
<xml_diff>
--- a/static/files/cadastre.xlsx
+++ b/static/files/cadastre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasoudard/workspace/beta.gouv.fr/appel/static/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D6468-AE64-0046-A33E-53A6891646EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5DF01B-7FDC-884E-868A-EB3E700A4D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31060" yWindow="3060" windowWidth="27020" windowHeight="16440" xr2:uid="{5E94D4F8-9F67-BB48-B84E-2D90FAF38DE8}"/>
   </bookViews>
@@ -262,8 +262,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,7 +581,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>